<commit_message>
Updated version of HSI, Review and SIQ, as well as the RTM itself
</commit_message>
<xml_diff>
--- a/Input Documents/RTM.xlsx
+++ b/Input Documents/RTM.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D090C9-263C-4E40-BD76-45BF8522DA9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93555B2-61D7-4132-973A-CB77106548EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,46 +20,124 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Questions</t>
-  </si>
-  <si>
-    <t>Answers</t>
-  </si>
-  <si>
-    <t>Which one of the two modes specified will be the default mode during the "Welcome" phase?</t>
-  </si>
-  <si>
-    <t>Modes will be handled according to mode switch connected as input signal to the controller, if it's LOW enter mode one and if it's HIGH enter mode 2.</t>
-  </si>
-  <si>
-    <t>Could you pleae elaborate more on the tail function? How do you intend it to work?</t>
-  </si>
-  <si>
-    <t>Tail function LEDs shall be ON when the Tail signal is HIGH level and shall be OFF when Tail signal level is LOW, activation and deactivation shall be done without any animation so simply ON all Tail LEDs when Tail signal is HIGH and OFF them when it's LOW. NOTE: Tail signal is provided by a switch connected as an input to the controller</t>
-  </si>
-  <si>
-    <t>Which switch will be used? where is their location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You have 4 switches:
-1- Tail switch to activate / deactivate Tail LEDs
-2- Right TI switch to activate / deactivate right TI LEDs 
-3- left TI switch to activate / deactivate left TI LEDs 
-4- Mode switch to select animation welcome mode
-All switches are connected as an input for the controller
-</t>
-  </si>
-  <si>
-    <t>How much do you need the delay in the animations to be?</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+  <si>
+    <t>CYRS</t>
+  </si>
+  <si>
+    <t>SRS</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ LED STRING ANIMATION_01_V01</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Req_ PO5_LSAN_ SRS_Start animation mode 1_01-V01</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ SRS_ Start animation mode 1_02-V01</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ SRS_ Start animation mode 1_03-V01</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ LED STRING ANIMATION_02_V01</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ LED STRING ANIMATION_03_V01</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ LED STRING ANIMATION_04_V01</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ LED STRING ANIMATION_05_V01</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ LED STRING ANIMATION_05_V02</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ LED STRING ANIMATION_05_V03</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ LED STRING ANIMATION_05_V04</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Req_ PO5_LSAN_ SRS_ Left Turn Indicator Off_01-V01</t>
+    </r>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ SRS_ Left Turn Indicator Off_01-V01</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ SRS_Left Turn Indicator On_02-V01</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ SRS_Left Turn Indicator On_03-V01</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ SRS_Left Turn Indicator On_01-V01</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ SRS_Right Turn Indicator On_03-V01</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ SRS_Right Turn Indicator On_02-V01</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ SRS_Right Turn Indicator Off_01-V01</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ SRS_Right Turn Indicator On_01-V01</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ SRS_Tail Function Low _03-V01</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ SRS_Tail Function Low _02-V01</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ SRS_Tail Function Low_01-V01</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ SRS_Tail Function High _03-V01</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ SRS_Tail Function High _02-V01</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ SRS_Tail Function High_01-V01</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ SRS_ Start animation mode 2_03-V01</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ SRS_ Start animation mode 2_02-V01</t>
+  </si>
+  <si>
+    <t>Req_ PO5_LSAN_ SRS_Start animation mode 2_01-V01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,13 +148,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF202124"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -96,13 +167,39 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,12 +211,29 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="5"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="5"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -128,22 +242,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -163,9 +292,9 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="1"/>
-        <name val="Arial"/>
+        <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -181,9 +310,9 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="1"/>
-        <name val="Arial"/>
+        <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -199,9 +328,9 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="11"/>
         <color theme="1"/>
-        <name val="Arial"/>
+        <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -238,11 +367,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B5" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" headerRowCellStyle="Neutral">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B5" totalsRowShown="0" headerRowDxfId="3" dataDxfId="0" headerRowCellStyle="Neutral">
   <autoFilter ref="A1:B5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Questions" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Answers" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="CYRS" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="SRS" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -511,69 +640,196 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="69.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="88.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="69.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="88.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="63" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="10"/>
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+    </row>
+    <row r="6" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B7" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="8"/>
+      <c r="B8" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="7"/>
+      <c r="B9" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="7"/>
+      <c r="B12" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="7"/>
+      <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="6"/>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
+      <c r="B15" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="7"/>
+      <c r="B16" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="7"/>
+      <c r="B17" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="7"/>
+      <c r="B20" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="7"/>
+      <c r="B21" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="7"/>
+      <c r="B24" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="7"/>
+      <c r="B25" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="6"/>
+      <c r="B28" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="6"/>
+      <c r="B29" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="6"/>
+      <c r="B32" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="6"/>
+      <c r="B33" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>